<commit_message>
changed some copy after discussion with BA
</commit_message>
<xml_diff>
--- a/docs/Copy of Results page copy- April 2017.xlsx
+++ b/docs/Copy of Results page copy- April 2017.xlsx
@@ -16,25 +16,25 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A11">
+    <comment authorId="0" ref="A12">
       <text>
         <t xml:space="preserve">Signed off 07/04
 	-Rhys Hobbs</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G10">
+    <comment authorId="0" ref="G11">
       <text>
         <t xml:space="preserve">Changed 'you business to 'your business' singed off 07/04
 	-Rhys Hobbs</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L12">
+    <comment authorId="0" ref="L13">
       <text>
         <t xml:space="preserve">Sign off on April 6th of the declaration copy
 	-Victoria Kio</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J10">
+    <comment authorId="0" ref="J11">
       <text>
         <t xml:space="preserve">reflecting the business
 	-Victoria Kio
@@ -47,7 +47,7 @@
 	-Victoria Kio</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K10">
+    <comment authorId="0" ref="K11">
       <text>
         <t xml:space="preserve">If you require further assistance call. 
 You can also review the Links to the ESM to help
@@ -63,7 +63,7 @@
 	-Victoria Kio</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I9">
+    <comment authorId="0" ref="I10">
       <text>
         <t xml:space="preserve">reflect the changes to all the rows were applicable to employed
 	-Victoria Kio
@@ -93,7 +93,7 @@
 	-Rhys Hobbs</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H8">
+    <comment authorId="0" ref="H9">
       <text>
         <t xml:space="preserve">remove bearing the running costs
 	-Victoria Kio
@@ -128,7 +128,7 @@
 	-Rhys Hobbs</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G7">
+    <comment authorId="0" ref="G8">
       <text>
         <t xml:space="preserve">remove significant
 	-Victoria Kio
@@ -163,7 +163,7 @@
 	-Rhys Hobbs</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L10">
+    <comment authorId="0" ref="L11">
       <text>
         <t xml:space="preserve">For the Public Sector, do we need to add in a step here for the end client to advise the agency/fee payer to operate PAYE?
 	-Francis Grant
@@ -208,7 +208,7 @@
 	-Rhys Hobbs</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E11">
+    <comment authorId="0" ref="E12">
       <text>
         <t xml:space="preserve">This is a hard exit outside IR35 so the comment saying IR35 applies is wrong.
 	-Francis Grant
@@ -229,7 +229,7 @@
 	-Rhys Hobbs</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E10">
+    <comment authorId="0" ref="E11">
       <text>
         <t xml:space="preserve">Are we confusing "worker" and "PSC"?
 	-Francis Grant
@@ -250,7 +250,7 @@
 	-Rhys Hobbs</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C11">
+    <comment authorId="0" ref="C12">
       <text>
         <t xml:space="preserve">Do we need "...of this transaction for security reasons"?
 	-Francis Grant
@@ -268,7 +268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="101">
   <si>
     <t>Result outcome (text for internal reference only) &gt;</t>
   </si>
@@ -371,7 +371,151 @@
     <t>Q&amp;A summary, including explanation</t>
   </si>
   <si>
-    <t>[Insert question, guidance and 'Yes' answer. No additional explanation needed.]</t>
+    <r>
+      <t xml:space="preserve">About the people involved
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FFB7B7B7"/>
+      </rPr>
+      <t xml:space="preserve">[Insert questions, guidance] </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">About the people involved
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FFB7B7B7"/>
+      </rPr>
+      <t xml:space="preserve">[Insert questions, guidance] </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">About the people involved
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FFB7B7B7"/>
+      </rPr>
+      <t xml:space="preserve">[Insert questions, guidance] </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">About the people involved
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FFB7B7B7"/>
+      </rPr>
+      <t xml:space="preserve">[Insert questions, guidance] </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">About the people involved
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FFB7B7B7"/>
+      </rPr>
+      <t xml:space="preserve">[Insert questions, guidance] </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">About the people involved
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FFB7B7B7"/>
+      </rPr>
+      <t xml:space="preserve">[Insert questions, guidance] </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">About the people involved
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FFB7B7B7"/>
+      </rPr>
+      <t xml:space="preserve">[Insert questions, guidance] </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">About the people involved
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FFB7B7B7"/>
+      </rPr>
+      <t xml:space="preserve">[Insert questions, guidance] </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">About the people involved
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FFB7B7B7"/>
+      </rPr>
+      <t xml:space="preserve">[Insert questions, guidance] </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">About the people involved
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FFB7B7B7"/>
+      </rPr>
+      <t xml:space="preserve">[Insert questions, guidance] </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve">About the worker’s duties
+</t>
+    </r>
+    <r>
+      <t>[Insert question, guidance and 'Yes' answer. No additional explanation needed.]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve">About the worker’s duties
+</t>
+    </r>
+    <r>
+      <t xml:space="preserve">
+[Insert question, guidance and 'Yes' answer. No additional explanation needed.]</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1147,8 +1291,7 @@
 If you require further assistance, please contact HMRC’s Employment Status and Intermediaries helpline for advice:
 - by phone on 0300 123 2326
 - by email at ir35@hmrc.gov.uk
-You could also read through the following link(s) in the Employment status manual 
-[https://www.gov.uk/hmrc-internal-manuals/employment-status-manual/esm0500]
+You could also read through the &lt;a href="https://www.gov.uk/hmrc-internal-manuals/employment-status-manual/esm0500"&gt;Employment status manual&lt;/a&gt; 
 </t>
     </r>
   </si>
@@ -1381,7 +1524,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1405,6 +1548,12 @@
     <font>
       <sz val="12.0"/>
       <color rgb="FF999999"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1455,7 +1604,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -1492,6 +1641,9 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1499,6 +1651,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1529,7 +1684,8 @@
     <col customWidth="1" min="2" max="2" width="5.71"/>
     <col customWidth="1" min="3" max="3" width="39.14"/>
     <col customWidth="1" min="4" max="4" width="40.14"/>
-    <col customWidth="1" min="5" max="6" width="42.86"/>
+    <col customWidth="1" min="5" max="5" width="50.14"/>
+    <col customWidth="1" min="6" max="6" width="42.86"/>
     <col customWidth="1" min="7" max="7" width="34.0"/>
     <col customWidth="1" min="8" max="8" width="35.43"/>
     <col customWidth="1" min="9" max="9" width="29.14"/>
@@ -1727,41 +1883,41 @@
       <c r="AB4" s="11"/>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="E5" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="I5" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="J5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="K5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="13"/>
+      <c r="L5" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="15"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
@@ -1780,36 +1936,40 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="14" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="E6" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="F6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="G6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="H6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="I6" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="J6" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="M6" s="11"/>
+      <c r="K6" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="15"/>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
@@ -1828,30 +1988,34 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" s="8" t="s">
+      <c r="E7" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="F7" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="G7" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="H7" s="16" t="s">
         <v>54</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>58</v>
       </c>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
@@ -1872,28 +2036,30 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="11"/>
+      <c r="G8" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="H8" s="8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
@@ -1914,7 +2080,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1922,18 +2088,20 @@
       <c r="E9" s="8"/>
       <c r="F9" s="9"/>
       <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="H9" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="I9" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
@@ -1954,27 +2122,15 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>72</v>
-      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="8" t="s">
         <v>73</v>
       </c>
@@ -2065,31 +2221,31 @@
         <v>89</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -2109,18 +2265,40 @@
       <c r="AB12" s="11"/>
     </row>
     <row r="13">
-      <c r="A13" s="6"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
+      <c r="A13" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
@@ -2619,7 +2797,7 @@
       <c r="AB29" s="11"/>
     </row>
     <row r="30">
-      <c r="A30" s="11"/>
+      <c r="A30" s="6"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -31898,6 +32076,36 @@
       <c r="AA1005" s="11"/>
       <c r="AB1005" s="11"/>
     </row>
+    <row r="1006">
+      <c r="A1006" s="11"/>
+      <c r="B1006" s="11"/>
+      <c r="C1006" s="11"/>
+      <c r="D1006" s="11"/>
+      <c r="E1006" s="11"/>
+      <c r="F1006" s="11"/>
+      <c r="G1006" s="11"/>
+      <c r="H1006" s="11"/>
+      <c r="I1006" s="11"/>
+      <c r="J1006" s="11"/>
+      <c r="K1006" s="11"/>
+      <c r="L1006" s="11"/>
+      <c r="M1006" s="11"/>
+      <c r="N1006" s="11"/>
+      <c r="O1006" s="11"/>
+      <c r="P1006" s="11"/>
+      <c r="Q1006" s="11"/>
+      <c r="R1006" s="11"/>
+      <c r="S1006" s="11"/>
+      <c r="T1006" s="11"/>
+      <c r="U1006" s="11"/>
+      <c r="V1006" s="11"/>
+      <c r="W1006" s="11"/>
+      <c r="X1006" s="11"/>
+      <c r="Y1006" s="11"/>
+      <c r="Z1006" s="11"/>
+      <c r="AA1006" s="11"/>
+      <c r="AB1006" s="11"/>
+    </row>
   </sheetData>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>